<commit_message>
Cucumber Day6 Apache poi
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liudmylakomisarenko/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liudmylakomisarenko/IdeaProjects/cybertek22-cucumber-junit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D395B6-D387-8047-B16A-4A3FB4AF1400}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69620E5D-9799-9B47-8544-51A6A4A99279}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{0F1184AB-A032-4C45-B3E3-B477020F874A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FirstName</t>
   </si>
@@ -70,12 +70,16 @@
   </si>
   <si>
     <t>SDET</t>
+  </si>
+  <si>
+    <t>Madam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -424,7 +428,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,7 +457,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>

</xml_diff>